<commit_message>
just need to add hours
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindsaycarbonell/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindsaycarbonell/Documents/REPOS/orange-elections/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="460" windowWidth="10000" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="36620" yWindow="8800" windowWidth="10000" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Anderson</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Seymour Senior Center</t>
+  </si>
+  <si>
+    <t>Campaign Funds</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +475,7 @@
     <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -482,8 +485,11 @@
       <c r="C1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -494,7 +500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -505,7 +511,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -513,7 +519,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -523,8 +529,11 @@
       <c r="C5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -534,8 +543,11 @@
       <c r="C6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>8442.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -545,8 +557,11 @@
       <c r="C7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>6761</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -556,8 +571,11 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -567,16 +585,22 @@
       <c r="C9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>20721</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -586,8 +610,11 @@
       <c r="C11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>3127.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -597,8 +624,11 @@
       <c r="C12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -608,8 +638,11 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>5163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>

</xml_diff>